<commit_message>
19/01/2025 maintenance sekolah & kategori kelas
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
   <si>
     <t>No</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>R = Menampilkan 3 Tabel dari 1 pengajar, tabel Gaji, tabel Transport, tabel Gaji custom, setiap tabel di lengkapi dengan button verifikasi</t>
+  </si>
+  <si>
+    <t>Catatan Maintenance DB</t>
+  </si>
+  <si>
+    <t>pembayaran_kelas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dibuat otomatis, saat menginput siswa, sistem langsung membuat juga tabel tagihan pembayaran secara otomatis, nantinya admin tinggal melakukan validasi pembayaran </t>
+  </si>
+  <si>
+    <t>jadi tidak usah ada fitur tambah pembayaran</t>
   </si>
 </sst>
 </file>
@@ -98,7 +110,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +129,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -182,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,13 +228,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -608,8 +629,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
@@ -618,8 +639,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
@@ -628,8 +649,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
@@ -734,24 +755,24 @@
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
@@ -770,7 +791,7 @@
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="9" t="s">
         <v>16</v>
       </c>
@@ -779,19 +800,40 @@
       </c>
       <c r="D23" s="8"/>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>